<commit_message>
ok test change password
</commit_message>
<xml_diff>
--- a/src/test/java/resources/Data_Test.xlsx
+++ b/src/test/java/resources/Data_Test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA3_TestAutomation\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D27F66-F69A-4EBE-9727-39E92B8D7613}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86063582-1382-4FFE-A00E-F1955BB4A9E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" activeTab="1" xr2:uid="{77DEAFC2-7D4F-4F22-A898-29ED0DE5A4F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" activeTab="2" xr2:uid="{77DEAFC2-7D4F-4F22-A898-29ED0DE5A4F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Search" sheetId="2" r:id="rId2"/>
+    <sheet name="ChangePassword" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>username</t>
   </si>
@@ -80,13 +81,59 @@
   </si>
   <si>
     <t>Không tìm thấy bất kỳ kết quả nào với từ khóa trên.</t>
+  </si>
+  <si>
+    <t>Mật khẩu cũ</t>
+  </si>
+  <si>
+    <t>Mật khẩu mới</t>
+  </si>
+  <si>
+    <t>Xác nhận lại mật khẩu</t>
+  </si>
+  <si>
+    <t>ngthiquyen</t>
+  </si>
+  <si>
+    <t>ngthiquyen1</t>
+  </si>
+  <si>
+    <t>Mật khẩu không đúng</t>
+  </si>
+  <si>
+    <t>Xác nhận mật khẩu không khớp</t>
+  </si>
+  <si>
+    <t>ngthiquyen2</t>
+  </si>
+  <si>
+    <t>ngthiquyen3</t>
+  </si>
+  <si>
+    <t>Mật khẩu mới dài từ 6 đến 50 ký tự</t>
+  </si>
+  <si>
+    <t>ad1</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>Mật khẩu mới dài từ 6 đến 50 ký tự
+Xác nhận mật khẩu không khớp</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>Đổi password thành công</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +152,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,12 +184,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -541,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9002D27-2518-4DA5-9F4E-FF207E623BAE}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -611,4 +667,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A4ACB5-A324-447F-B65B-C86042D78515}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>